<commit_message>
Update upstream-downstream population calculation
</commit_message>
<xml_diff>
--- a/9_AridityDroughtResearch/6_TransboundaryBasinMetLandMeteorologicalChange/Basins_Up_Middle_Down_Statistical.xlsx
+++ b/9_AridityDroughtResearch/6_TransboundaryBasinMetLandMeteorologicalChange/Basins_Up_Middle_Down_Statistical.xlsx
@@ -1,111 +1,418 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CMIP6\Program\9_AridityDroughtResearch\6_TransboundaryBasinMetLandMeteorologicalChange\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDCAF59E-2528-47AC-B443-2663F568A4CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4710" yWindow="3960" windowWidth="21600" windowHeight="13185" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="24315" windowHeight="14790" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Extent" sheetId="1" r:id="rId1"/>
     <sheet name="Intensity" sheetId="2" r:id="rId2"/>
     <sheet name="Frequency" sheetId="3" r:id="rId3"/>
+    <sheet name="ExposedPopulation" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="12">
   <si>
     <t>Historical(1951-2000)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>SSP126(2001-2050)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>SSP245(2001-2050)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>SSP370(2001-2050)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>SSP585(2001-2050)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>SSP126(2051-2100)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>SSP245(2051-2100)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>SSP370(2051-2100)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>SSP585(2051-2100)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Up</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Middle</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Down</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
-      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
-      <family val="3"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -128,32 +435,318 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
@@ -173,7 +766,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr lang="zh-CN" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -193,6 +786,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -201,26 +795,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -253,6 +827,9 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Extent!$B$1:$J$1</c:f>
@@ -295,40 +872,35 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>12.790287017822266</c:v>
+                  <c:v>12.7902870178223</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.776620864868164</c:v>
+                  <c:v>17.7766208648682</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.747190475463867</c:v>
+                  <c:v>17.7471904754639</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.590143203735352</c:v>
+                  <c:v>17.5901432037354</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18.097396850585938</c:v>
+                  <c:v>18.0973968505859</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.987194061279297</c:v>
+                  <c:v>20.9871940612793</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22.934198379516602</c:v>
+                  <c:v>22.9341983795166</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26.260835647583008</c:v>
+                  <c:v>26.260835647583</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>27.462245941162109</c:v>
+                  <c:v>27.4622459411621</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-BF24-4EAA-83E9-35F17F2D1A9F}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -354,6 +926,9 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Extent!$B$1:$J$1</c:f>
@@ -396,40 +971,35 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>12.150692939758301</c:v>
+                  <c:v>12.1506929397583</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.846684455871582</c:v>
+                  <c:v>14.8466844558716</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.790637016296387</c:v>
+                  <c:v>14.7906370162964</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>14.74365234375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15.034157752990723</c:v>
+                  <c:v>15.0341577529907</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.567529678344727</c:v>
+                  <c:v>17.5675296783447</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18.935314178466797</c:v>
+                  <c:v>18.9353141784668</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20.865612030029297</c:v>
+                  <c:v>20.8656120300293</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>22.238391876220703</c:v>
+                  <c:v>22.2383918762207</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-BF24-4EAA-83E9-35F17F2D1A9F}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -455,6 +1025,9 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Extent!$B$1:$J$1</c:f>
@@ -497,40 +1070,35 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>10.237793922424316</c:v>
+                  <c:v>10.2377939224243</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.168244361877441</c:v>
+                  <c:v>14.1682443618774</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.283552169799805</c:v>
+                  <c:v>14.2835521697998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14.388184547424316</c:v>
+                  <c:v>14.3881845474243</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15.077066421508789</c:v>
+                  <c:v>15.0770664215088</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.128149032592773</c:v>
+                  <c:v>17.1281490325928</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>19.262939453125</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21.878566741943359</c:v>
+                  <c:v>21.8785667419434</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23.790002822875977</c:v>
+                  <c:v>23.790002822876</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-BF24-4EAA-83E9-35F17F2D1A9F}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -574,7 +1142,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -586,7 +1154,6 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2093477072"/>
@@ -633,7 +1200,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -645,7 +1212,6 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2093476240"/>
@@ -662,6 +1228,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -675,7 +1242,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr lang="zh-CN" sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -687,19 +1254,11 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -722,9 +1281,8 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr lang="zh-CN"/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -736,7 +1294,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
@@ -756,7 +1314,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr lang="zh-CN" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -772,9 +1330,11 @@
               <a:rPr lang="en-US" altLang="zh-CN"/>
               <a:t>Intensity</a:t>
             </a:r>
+            <a:endParaRPr lang="en-US" altLang="zh-CN"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -783,26 +1343,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -835,6 +1375,9 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Intensity!$B$1:$J$1</c:f>
@@ -877,40 +1420,35 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>5.5204463652576301E-2</c:v>
+                  <c:v>0.0552044636525763</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.9090291693161739E-2</c:v>
+                  <c:v>0.0590902916931617</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.9179007325891889E-2</c:v>
+                  <c:v>0.0591790073258919</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.9235777570094753E-2</c:v>
+                  <c:v>0.0592357775700948</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.9604329342653653E-2</c:v>
+                  <c:v>0.0596043293426537</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.1555328303104707E-2</c:v>
+                  <c:v>0.0615553283031047</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.325503253647341E-2</c:v>
+                  <c:v>0.0632550325364734</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.5536422412096618E-2</c:v>
+                  <c:v>0.0655364224120966</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.651474960558855E-2</c:v>
+                  <c:v>0.0665147496055885</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0819-4827-8395-1F943D263829}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -936,6 +1474,9 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Intensity!$B$1:$J$1</c:f>
@@ -978,40 +1519,35 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>5.5784482728726138E-2</c:v>
+                  <c:v>0.0557844827287261</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.9727208481241974E-2</c:v>
+                  <c:v>0.059727208481242</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.9847857769961842E-2</c:v>
+                  <c:v>0.0598478577699618</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0013202389969163E-2</c:v>
+                  <c:v>0.0600132023899692</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.0411967393243983E-2</c:v>
+                  <c:v>0.060411967393244</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.2157839649137549E-2</c:v>
+                  <c:v>0.0621578396491375</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.3903810789184556E-2</c:v>
+                  <c:v>0.0639038107891846</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.605154580341431E-2</c:v>
+                  <c:v>0.0660515458034143</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.7485110540949203E-2</c:v>
+                  <c:v>0.0674851105409492</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0819-4827-8395-1F943D263829}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1037,6 +1573,9 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Intensity!$B$1:$J$1</c:f>
@@ -1079,40 +1618,35 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>5.5457118303646864E-2</c:v>
+                  <c:v>0.0554571183036469</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.9652382814961095E-2</c:v>
+                  <c:v>0.0596523828149611</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.9758354506577335E-2</c:v>
+                  <c:v>0.0597583545065773</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.9761587058566004E-2</c:v>
+                  <c:v>0.059761587058566</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.0176241766733314E-2</c:v>
+                  <c:v>0.0601762417667333</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.2358555590160167E-2</c:v>
+                  <c:v>0.0623585555901602</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.3886677002769149E-2</c:v>
+                  <c:v>0.0638866770027691</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.6059946517664725E-2</c:v>
+                  <c:v>0.0660599465176647</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.7304610517617783E-2</c:v>
+                  <c:v>0.0673046105176178</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-0819-4827-8395-1F943D263829}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1156,7 +1690,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1168,7 +1702,6 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2093475824"/>
@@ -1215,7 +1748,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1227,7 +1760,6 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2093479152"/>
@@ -1244,6 +1776,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1257,7 +1790,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr lang="zh-CN" sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1269,19 +1802,11 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -1304,9 +1829,8 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr lang="zh-CN"/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1318,7 +1842,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
@@ -1338,7 +1862,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr lang="zh-CN" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1358,6 +1882,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1366,26 +1891,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1418,6 +1923,9 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Frequency!$B$1:$J$1</c:f>
@@ -1460,40 +1968,35 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1.7231421906003277</c:v>
+                  <c:v>1.72314219060033</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.7271836680475889</c:v>
+                  <c:v>2.72718366804759</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.731447642609858</c:v>
+                  <c:v>2.73144764260986</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.7259326123561372</c:v>
+                  <c:v>2.72593261235614</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.8627292425965747</c:v>
+                  <c:v>2.86272924259657</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.391477032154155</c:v>
+                  <c:v>3.39147703215415</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.963801047728952</c:v>
+                  <c:v>3.96380104772895</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.1077334351728085</c:v>
+                  <c:v>5.10773343517281</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.679658948452067</c:v>
+                  <c:v>5.67965894845207</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-0C95-4808-821F-71284B08D236}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1519,6 +2022,9 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Frequency!$B$1:$J$1</c:f>
@@ -1561,40 +2067,35 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1.590444681793316</c:v>
+                  <c:v>1.59044468179332</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.1934470002865556</c:v>
+                  <c:v>2.19344700028656</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2073058587542667</c:v>
+                  <c:v>2.20730585875427</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.2138746663761646</c:v>
+                  <c:v>2.21387466637616</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.3092804855810565</c:v>
+                  <c:v>2.30928048558106</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.7374918592231738</c:v>
+                  <c:v>2.73749185922317</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.1653072654805015</c:v>
+                  <c:v>3.1653072654805</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>3.94006890353505</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.5178979862974451</c:v>
+                  <c:v>4.51789798629745</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0C95-4808-821F-71284B08D236}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1620,6 +2121,9 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Frequency!$B$1:$J$1</c:f>
@@ -1662,40 +2166,35 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1.3372031495176513</c:v>
+                  <c:v>1.33720314951765</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0634779794113292</c:v>
+                  <c:v>2.06347797941133</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0970158390621814</c:v>
+                  <c:v>2.09701583906218</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.1285453662699165</c:v>
+                  <c:v>2.12854536626992</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.297081278101845</c:v>
+                  <c:v>2.29708127810184</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.6200123841623451</c:v>
+                  <c:v>2.62001238416234</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.1196514139758085</c:v>
+                  <c:v>3.11965141397581</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.0247782077123411</c:v>
+                  <c:v>4.02477820771234</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.7591329679067247</c:v>
+                  <c:v>4.75913296790672</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-0C95-4808-821F-71284B08D236}"/>
-            </c:ext>
-          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1739,7 +2238,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1751,7 +2250,6 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2118427664"/>
@@ -1798,7 +2296,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1810,7 +2308,6 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2118433488"/>
@@ -1827,6 +2324,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1840,7 +2338,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr lang="zh-CN" sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1852,19 +2350,11 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -1887,9 +2377,556 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr lang="zh-CN"/>
       </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN"/>
+              <a:t>Frequency</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ExposedPopulation!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Up</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>ExposedPopulation!$B$1:$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Historical(1951-2000)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SSP126(2001-2050)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SSP245(2001-2050)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>SSP370(2001-2050)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SSP585(2001-2050)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>SSP126(2051-2100)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>SSP245(2051-2100)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>SSP370(2051-2100)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SSP585(2051-2100)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ExposedPopulation!$B$2:$J$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>51448067.7269565</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>76820694.9452174</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>78626634.9347826</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80325507.3918182</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>76846992.6347826</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>94753026.2286957</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>120605065.834783</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>171390256.292727</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>134383301.56087</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ExposedPopulation!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Middle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>ExposedPopulation!$B$1:$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Historical(1951-2000)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SSP126(2001-2050)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SSP245(2001-2050)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>SSP370(2001-2050)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SSP585(2001-2050)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>SSP126(2051-2100)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>SSP245(2051-2100)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>SSP370(2051-2100)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SSP585(2051-2100)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ExposedPopulation!$B$3:$J$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>49560156.9295652</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>69632587.273913</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70496897.1217391</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70110875.4090909</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>67067768.7826087</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>104620523.532174</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>137072322.233913</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>187450731.288182</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>134698443.133913</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ExposedPopulation!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Down</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>ExposedPopulation!$B$1:$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Historical(1951-2000)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>SSP126(2001-2050)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>SSP245(2001-2050)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>SSP370(2001-2050)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>SSP585(2001-2050)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>SSP126(2051-2100)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>SSP245(2051-2100)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>SSP370(2051-2100)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SSP585(2051-2100)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ExposedPopulation!$B$4:$J$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>95361300.426087</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>116961232.371304</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>119997976.007826</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120498513.993636</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>119877958.66</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>139757617.149565</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>178919997.587826</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>231919793.326364</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>207478994.426087</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="2118433488"/>
+        <c:axId val="2118427664"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2118433488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2118427664"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2118427664"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="zh-CN" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2118433488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="zh-CN" sz="1500" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr lang="zh-CN"/>
+      </a:pPr>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2020,6 +3057,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -3531,8 +4608,511 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
@@ -3546,20 +5126,14 @@
       <xdr:row>33</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
+    <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="图表 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE109D3C-648A-4670-9025-DCF8587C7A2B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="3" name="图表 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off x="3495675" y="1790700"/>
+        <a:ext cx="7772400" cy="4267200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3573,34 +5147,28 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1504949</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:colOff>1418590</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>27940</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>781049</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>76199</xdr:rowOff>
+      <xdr:colOff>694690</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>27940</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
+    <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="图表 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{417E793A-5B38-4D8E-BAC5-4436934F10C8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="图表 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off x="2104390" y="3285490"/>
+        <a:ext cx="9191625" cy="3800475"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3614,7 +5182,7 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
@@ -3628,20 +5196,49 @@
       <xdr:row>34</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame macro="">
+    <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="图表 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DD99B85-420C-460A-911A-B81EC89E0409}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="图表 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
+        <a:off x="2857500" y="1628775"/>
+        <a:ext cx="9410700" cy="4638675"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="图表 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="2857500" y="1628775"/>
+        <a:ext cx="9410700" cy="4638675"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3697,7 +5294,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -3732,7 +5329,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -3906,30 +5503,25 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4:J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6"/>
   <cols>
-    <col min="2" max="2" width="19.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.875" customWidth="1"/>
+    <col min="3" max="10" width="18.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -3959,125 +5551,228 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1">
-        <v>12.790287017822266</v>
+        <v>12.7902870178223</v>
       </c>
       <c r="C2" s="1">
-        <v>17.776620864868164</v>
+        <v>17.7766208648682</v>
       </c>
       <c r="D2" s="1">
-        <v>17.747190475463867</v>
+        <v>17.7471904754639</v>
       </c>
       <c r="E2" s="1">
-        <v>17.590143203735352</v>
+        <v>17.5901432037354</v>
       </c>
       <c r="F2" s="1">
-        <v>18.097396850585938</v>
+        <v>18.0973968505859</v>
       </c>
       <c r="G2" s="1">
-        <v>20.987194061279297</v>
+        <v>20.9871940612793</v>
       </c>
       <c r="H2" s="1">
-        <v>22.934198379516602</v>
+        <v>22.9341983795166</v>
       </c>
       <c r="I2" s="1">
-        <v>26.260835647583008</v>
+        <v>26.260835647583</v>
       </c>
       <c r="J2" s="1">
-        <v>27.462245941162109</v>
+        <v>27.4622459411621</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1">
-        <v>12.150692939758301</v>
+        <v>12.1506929397583</v>
       </c>
       <c r="C3" s="1">
-        <v>14.846684455871582</v>
+        <v>14.8466844558716</v>
       </c>
       <c r="D3" s="1">
-        <v>14.790637016296387</v>
+        <v>14.7906370162964</v>
       </c>
       <c r="E3" s="1">
         <v>14.74365234375</v>
       </c>
       <c r="F3" s="1">
-        <v>15.034157752990723</v>
+        <v>15.0341577529907</v>
       </c>
       <c r="G3" s="1">
-        <v>17.567529678344727</v>
+        <v>17.5675296783447</v>
       </c>
       <c r="H3" s="1">
-        <v>18.935314178466797</v>
+        <v>18.9353141784668</v>
       </c>
       <c r="I3" s="1">
-        <v>20.865612030029297</v>
+        <v>20.8656120300293</v>
       </c>
       <c r="J3" s="1">
-        <v>22.238391876220703</v>
+        <v>22.2383918762207</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1">
-        <v>10.237793922424316</v>
+        <v>10.2377939224243</v>
       </c>
       <c r="C4" s="1">
-        <v>14.168244361877441</v>
+        <v>14.1682443618774</v>
       </c>
       <c r="D4" s="1">
-        <v>14.283552169799805</v>
+        <v>14.2835521697998</v>
       </c>
       <c r="E4" s="1">
-        <v>14.388184547424316</v>
+        <v>14.3881845474243</v>
       </c>
       <c r="F4" s="1">
-        <v>15.077066421508789</v>
+        <v>15.0770664215088</v>
       </c>
       <c r="G4" s="1">
-        <v>17.128149032592773</v>
+        <v>17.1281490325928</v>
       </c>
       <c r="H4" s="1">
         <v>19.262939453125</v>
       </c>
       <c r="I4" s="1">
-        <v>21.878566741943359</v>
+        <v>21.8785667419434</v>
       </c>
       <c r="J4" s="1">
-        <v>23.790002822875977</v>
+        <v>23.790002822876</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10">
+      <c r="C5">
+        <f>(C2-$B$2)/$B$2*100</f>
+        <v>38.9853162802198</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:J5" si="0">(D2-$B$2)/$B$2*100</f>
+        <v>38.7552167573296</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>37.5273532112678</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>41.4932817799056</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>64.0869671809185</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>79.3094896741534</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>105.318579723743</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>114.711725412382</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10">
+      <c r="C6">
+        <f>(C3-$B$3)/$B$3*100</f>
+        <v>22.1879651595155</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:J6" si="1">(D3-$B$3)/$B$3*100</f>
+        <v>21.7266956677007</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>21.3400125972015</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>23.730867264347</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>44.5804759073615</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>55.8373195038822</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>71.7236385898198</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>83.021593801078</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10">
+      <c r="C7">
+        <f>(C4-$B$4)/$B$4*100</f>
+        <v>38.3915760488603</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ref="D7:J7" si="2">(D4-$B$4)/$B$4*100</f>
+        <v>39.5178715066131</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>40.5398922507046</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>47.2687039390858</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>67.303123723522</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>88.1551787336966</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>113.703918126558</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>132.3743084022</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F62013-A7D5-484F-BC5F-F53767EEC4D9}">
-  <dimension ref="A1:J4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J4"/>
+      <selection activeCell="B4" sqref="B4:J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6"/>
   <cols>
-    <col min="2" max="2" width="19.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.875" customWidth="1"/>
+    <col min="3" max="10" width="18.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -4107,124 +5802,227 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1">
-        <v>5.5204463652576301E-2</v>
+        <v>0.0552044636525763</v>
       </c>
       <c r="C2" s="1">
-        <v>5.9090291693161739E-2</v>
+        <v>0.0590902916931617</v>
       </c>
       <c r="D2" s="1">
-        <v>5.9179007325891889E-2</v>
+        <v>0.0591790073258919</v>
       </c>
       <c r="E2" s="1">
-        <v>5.9235777570094753E-2</v>
+        <v>0.0592357775700948</v>
       </c>
       <c r="F2" s="1">
-        <v>5.9604329342653653E-2</v>
+        <v>0.0596043293426537</v>
       </c>
       <c r="G2" s="1">
-        <v>6.1555328303104707E-2</v>
+        <v>0.0615553283031047</v>
       </c>
       <c r="H2" s="1">
-        <v>6.325503253647341E-2</v>
+        <v>0.0632550325364734</v>
       </c>
       <c r="I2" s="1">
-        <v>6.5536422412096618E-2</v>
+        <v>0.0655364224120966</v>
       </c>
       <c r="J2" s="1">
-        <v>6.651474960558855E-2</v>
+        <v>0.0665147496055885</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1">
-        <v>5.5784482728726138E-2</v>
+        <v>0.0557844827287261</v>
       </c>
       <c r="C3" s="1">
-        <v>5.9727208481241974E-2</v>
+        <v>0.059727208481242</v>
       </c>
       <c r="D3" s="1">
-        <v>5.9847857769961842E-2</v>
+        <v>0.0598478577699618</v>
       </c>
       <c r="E3" s="1">
-        <v>6.0013202389969163E-2</v>
+        <v>0.0600132023899692</v>
       </c>
       <c r="F3" s="1">
-        <v>6.0411967393243983E-2</v>
+        <v>0.060411967393244</v>
       </c>
       <c r="G3" s="1">
-        <v>6.2157839649137549E-2</v>
+        <v>0.0621578396491375</v>
       </c>
       <c r="H3" s="1">
-        <v>6.3903810789184556E-2</v>
+        <v>0.0639038107891846</v>
       </c>
       <c r="I3" s="1">
-        <v>6.605154580341431E-2</v>
+        <v>0.0660515458034143</v>
       </c>
       <c r="J3" s="1">
-        <v>6.7485110540949203E-2</v>
+        <v>0.0674851105409492</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1">
-        <v>5.5457118303646864E-2</v>
+        <v>0.0554571183036469</v>
       </c>
       <c r="C4" s="1">
-        <v>5.9652382814961095E-2</v>
+        <v>0.0596523828149611</v>
       </c>
       <c r="D4" s="1">
-        <v>5.9758354506577335E-2</v>
+        <v>0.0597583545065773</v>
       </c>
       <c r="E4" s="1">
-        <v>5.9761587058566004E-2</v>
+        <v>0.059761587058566</v>
       </c>
       <c r="F4" s="1">
-        <v>6.0176241766733314E-2</v>
+        <v>0.0601762417667333</v>
       </c>
       <c r="G4" s="1">
-        <v>6.2358555590160167E-2</v>
+        <v>0.0623585555901602</v>
       </c>
       <c r="H4" s="1">
-        <v>6.3886677002769149E-2</v>
+        <v>0.0638866770027691</v>
       </c>
       <c r="I4" s="1">
-        <v>6.6059946517664725E-2</v>
+        <v>0.0660599465176647</v>
       </c>
       <c r="J4" s="1">
-        <v>6.7304610517617783E-2</v>
+        <v>0.0673046105176178</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10">
+      <c r="C5">
+        <f t="shared" ref="C5:J5" si="0">(C2-$B$2)/$B$2*100</f>
+        <v>7.03897435729202</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>7.19967808822304</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>7.30251441783606</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>7.97012668715969</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>11.5042593122486</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>14.5831846760844</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>18.7158031722642</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>20.4879917395673</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10">
+      <c r="C6">
+        <f t="shared" ref="C6:J6" si="1">(C3-$B$3)/$B$3*100</f>
+        <v>7.06778222124758</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>7.28405972857264</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>7.5804586766661</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>8.29529008455774</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>11.4249637330229</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>14.5548146425267</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>18.4048727754917</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>20.974699844618</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10">
+      <c r="C7">
+        <f t="shared" ref="C7:J7" si="2">(C4-$B$4)/$B$4*100</f>
+        <v>7.56488010852585</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>7.75596773597163</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>7.7617966576458</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>8.50949996580713</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>12.4446374020474</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>15.2001383356552</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>19.1189671197189</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>21.3633390561367</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98736918-6861-4E43-8803-5D5FF00730C6}">
-  <dimension ref="A1:J4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6"/>
   <cols>
-    <col min="2" max="2" width="19.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.875" customWidth="1"/>
+    <col min="3" max="10" width="18.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -4254,105 +6052,457 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1">
-        <v>1.7231421906003277</v>
+        <v>1.72314219060033</v>
       </c>
       <c r="C2" s="1">
-        <v>2.7271836680475889</v>
+        <v>2.72718366804759</v>
       </c>
       <c r="D2" s="1">
-        <v>2.731447642609858</v>
+        <v>2.73144764260986</v>
       </c>
       <c r="E2" s="1">
-        <v>2.7259326123561372</v>
+        <v>2.72593261235614</v>
       </c>
       <c r="F2" s="1">
-        <v>2.8627292425965747</v>
+        <v>2.86272924259657</v>
       </c>
       <c r="G2" s="1">
-        <v>3.391477032154155</v>
+        <v>3.39147703215415</v>
       </c>
       <c r="H2" s="1">
-        <v>3.963801047728952</v>
+        <v>3.96380104772895</v>
       </c>
       <c r="I2" s="1">
-        <v>5.1077334351728085</v>
+        <v>5.10773343517281</v>
       </c>
       <c r="J2" s="1">
-        <v>5.679658948452067</v>
+        <v>5.67965894845207</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1">
-        <v>1.590444681793316</v>
+        <v>1.59044468179332</v>
       </c>
       <c r="C3" s="1">
-        <v>2.1934470002865556</v>
+        <v>2.19344700028656</v>
       </c>
       <c r="D3" s="1">
-        <v>2.2073058587542667</v>
+        <v>2.20730585875427</v>
       </c>
       <c r="E3" s="1">
-        <v>2.2138746663761646</v>
+        <v>2.21387466637616</v>
       </c>
       <c r="F3" s="1">
-        <v>2.3092804855810565</v>
+        <v>2.30928048558106</v>
       </c>
       <c r="G3" s="1">
-        <v>2.7374918592231738</v>
+        <v>2.73749185922317</v>
       </c>
       <c r="H3" s="1">
-        <v>3.1653072654805015</v>
+        <v>3.1653072654805</v>
       </c>
       <c r="I3" s="1">
         <v>3.94006890353505</v>
       </c>
       <c r="J3" s="1">
-        <v>4.5178979862974451</v>
+        <v>4.51789798629745</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1">
-        <v>1.3372031495176513</v>
+        <v>1.33720314951765</v>
       </c>
       <c r="C4" s="1">
-        <v>2.0634779794113292</v>
+        <v>2.06347797941133</v>
       </c>
       <c r="D4" s="1">
-        <v>2.0970158390621814</v>
+        <v>2.09701583906218</v>
       </c>
       <c r="E4" s="1">
-        <v>2.1285453662699165</v>
+        <v>2.12854536626992</v>
       </c>
       <c r="F4" s="1">
-        <v>2.297081278101845</v>
+        <v>2.29708127810184</v>
       </c>
       <c r="G4" s="1">
-        <v>2.6200123841623451</v>
+        <v>2.62001238416234</v>
       </c>
       <c r="H4" s="1">
-        <v>3.1196514139758085</v>
+        <v>3.11965141397581</v>
       </c>
       <c r="I4" s="1">
-        <v>4.0247782077123411</v>
+        <v>4.02477820771234</v>
       </c>
       <c r="J4" s="1">
-        <v>4.7591329679067247</v>
+        <v>4.75913296790672</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10">
+      <c r="C5">
+        <f t="shared" ref="C5:J5" si="0">(C2-$B$2)/$B$2*100</f>
+        <v>58.2680572110803</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>58.5155106473393</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>58.1954540505126</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>66.1342434891705</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>96.8193368286452</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>130.03331178073</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>196.419730364406</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>229.610578827121</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10">
+      <c r="C6">
+        <f t="shared" ref="C6:J6" si="1">(C3-$B$3)/$B$3*100</f>
+        <v>37.9140705361296</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>38.7854531517189</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>39.1984701963916</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>45.1971585064633</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>72.1211614940607</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>99.0202678354986</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>147.733790973</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>184.065081798586</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10">
+      <c r="C7">
+        <f t="shared" ref="C7:J7" si="2">(C4-$B$4)/$B$4*100</f>
+        <v>54.3129763159514</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>56.8210364908732</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>59.1789076355163</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>71.7825207733347</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>95.9322624320337</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>133.296744410235</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>200.984798694509</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>255.902016056679</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6"/>
+  <cols>
+    <col min="2" max="2" width="19.875" customWidth="1"/>
+    <col min="3" max="10" width="18.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1">
+        <v>51448067.7269565</v>
+      </c>
+      <c r="C2" s="1">
+        <v>76820694.9452174</v>
+      </c>
+      <c r="D2" s="1">
+        <v>78626634.9347826</v>
+      </c>
+      <c r="E2" s="1">
+        <v>80325507.3918182</v>
+      </c>
+      <c r="F2" s="1">
+        <v>76846992.6347826</v>
+      </c>
+      <c r="G2" s="1">
+        <v>94753026.2286957</v>
+      </c>
+      <c r="H2" s="1">
+        <v>120605065.834783</v>
+      </c>
+      <c r="I2" s="1">
+        <v>171390256.292727</v>
+      </c>
+      <c r="J2" s="1">
+        <v>134383301.56087</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1">
+        <v>49560156.9295652</v>
+      </c>
+      <c r="C3" s="1">
+        <v>69632587.273913</v>
+      </c>
+      <c r="D3" s="1">
+        <v>70496897.1217391</v>
+      </c>
+      <c r="E3" s="1">
+        <v>70110875.4090909</v>
+      </c>
+      <c r="F3" s="1">
+        <v>67067768.7826087</v>
+      </c>
+      <c r="G3" s="1">
+        <v>104620523.532174</v>
+      </c>
+      <c r="H3" s="1">
+        <v>137072322.233913</v>
+      </c>
+      <c r="I3" s="1">
+        <v>187450731.288182</v>
+      </c>
+      <c r="J3" s="1">
+        <v>134698443.133913</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1">
+        <v>95361300.426087</v>
+      </c>
+      <c r="C4" s="1">
+        <v>116961232.371304</v>
+      </c>
+      <c r="D4" s="1">
+        <v>119997976.007826</v>
+      </c>
+      <c r="E4" s="1">
+        <v>120498513.993636</v>
+      </c>
+      <c r="F4" s="1">
+        <v>119877958.66</v>
+      </c>
+      <c r="G4" s="1">
+        <v>139757617.149565</v>
+      </c>
+      <c r="H4" s="1">
+        <v>178919997.587826</v>
+      </c>
+      <c r="I4" s="1">
+        <v>231919793.326364</v>
+      </c>
+      <c r="J4" s="1">
+        <v>207478994.426087</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10">
+      <c r="C5">
+        <f>(C2-$B$2)/$B$2*100</f>
+        <v>49.3169682346821</v>
+      </c>
+      <c r="D5">
+        <f>(D2-$B$2)/$B$2*100</f>
+        <v>52.8271875089018</v>
+      </c>
+      <c r="E5">
+        <f>(E2-$B$2)/$B$2*100</f>
+        <v>56.1292988069427</v>
+      </c>
+      <c r="F5">
+        <f>(F2-$B$2)/$B$2*100</f>
+        <v>49.3680832536267</v>
+      </c>
+      <c r="G5">
+        <f>(G2-$B$2)/$B$2*100</f>
+        <v>84.172176750283</v>
+      </c>
+      <c r="H5">
+        <f>(H2-$B$2)/$B$2*100</f>
+        <v>134.420982484423</v>
+      </c>
+      <c r="I5">
+        <f>(I2-$B$2)/$B$2*100</f>
+        <v>233.132542901949</v>
+      </c>
+      <c r="J5">
+        <f>(J2-$B$2)/$B$2*100</f>
+        <v>161.201843913875</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10">
+      <c r="C6">
+        <f>(C3-$B$3)/$B$3*100</f>
+        <v>40.5011436361566</v>
+      </c>
+      <c r="D6">
+        <f>(D3-$B$3)/$B$3*100</f>
+        <v>42.2451047157279</v>
+      </c>
+      <c r="E6">
+        <f>(E3-$B$3)/$B$3*100</f>
+        <v>41.4662094567866</v>
+      </c>
+      <c r="F6">
+        <f>(F3-$B$3)/$B$3*100</f>
+        <v>35.3259814691976</v>
+      </c>
+      <c r="G6">
+        <f>(G3-$B$3)/$B$3*100</f>
+        <v>111.098047330359</v>
+      </c>
+      <c r="H6">
+        <f>(H3-$B$3)/$B$3*100</f>
+        <v>176.577659809915</v>
+      </c>
+      <c r="I6">
+        <f>(I3-$B$3)/$B$3*100</f>
+        <v>278.228687924831</v>
+      </c>
+      <c r="J6">
+        <f>(J3-$B$3)/$B$3*100</f>
+        <v>171.787765574161</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10">
+      <c r="C7">
+        <f>(C4-$B$4)/$B$4*100</f>
+        <v>22.6506264582236</v>
+      </c>
+      <c r="D7">
+        <f>(D4-$B$4)/$B$4*100</f>
+        <v>25.8350876840596</v>
+      </c>
+      <c r="E7">
+        <f>(E4-$B$4)/$B$4*100</f>
+        <v>26.359973548214</v>
+      </c>
+      <c r="F7">
+        <f>(F4-$B$4)/$B$4*100</f>
+        <v>25.7092322822459</v>
+      </c>
+      <c r="G7">
+        <f>(G4-$B$4)/$B$4*100</f>
+        <v>46.555905304468</v>
+      </c>
+      <c r="H7">
+        <f>(H4-$B$4)/$B$4*100</f>
+        <v>87.6232777745141</v>
+      </c>
+      <c r="I7">
+        <f>(I4-$B$4)/$B$4*100</f>
+        <v>143.201164717884</v>
+      </c>
+      <c r="J7">
+        <f>(J4-$B$4)/$B$4*100</f>
+        <v>117.57148182653</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>